<commit_message>
se agrega campo sucursal en usuario y en ventas y compras ya respeta el inventario local por sucursal, faltan pruebas
</commit_message>
<xml_diff>
--- a/ejemploempleados.xlsx
+++ b/ejemploempleados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>usuario</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>4tcel</t>
+  </si>
+  <si>
+    <t>idSucursal</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +466,7 @@
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +491,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -514,8 +520,11 @@
       <c r="H2" t="s">
         <v>32</v>
       </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -540,8 +549,11 @@
       <c r="H3" t="s">
         <v>33</v>
       </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -566,8 +578,11 @@
       <c r="H4" t="s">
         <v>34</v>
       </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -591,9 +606,13 @@
       </c>
       <c r="H5" t="s">
         <v>35</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>